<commit_message>
Failing to parse JSON for shunk results
</commit_message>
<xml_diff>
--- a/doc/regression-test/suites/legacy-security/04-workflow.xlsx
+++ b/doc/regression-test/suites/legacy-security/04-workflow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\Dev\Propel\propel\doc\regression-test\suites\legacy-security\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5583EE5C-4D5B-4CC6-AE98-C106D154A24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB088DA-ECF9-4042-969C-746E754AFE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -605,6 +605,66 @@
 WHen the execution is done, you must be redirected to the Results page for the execution report.</t>
   </si>
   <si>
+    <t>Review the Execution report</t>
+  </si>
+  <si>
+    <t>Creating and executing a Workflow that generates as huge Payload</t>
+  </si>
+  <si>
+    <t>Cancelling a Workflow execution</t>
+  </si>
+  <si>
+    <t>For the first step all the 30K results need to be there in a paginated Table.   
+For the second step, you need to see a legend saying the maximum quota for the results was exceeded and the data was discarded.</t>
+  </si>
+  <si>
+    <t>You are redirected to the Browse Workflows page where the Workflow TestWorkflowHugeResults is visible in the workflow list.</t>
+  </si>
+  <si>
+    <t>In the Search textbox of the navigation bar type the word "huge" and press enter.</t>
+  </si>
+  <si>
+    <t>Click the Run button at the right of the Workflow name</t>
+  </si>
+  <si>
+    <t>The workflow execution starts</t>
+  </si>
+  <si>
+    <t>As soon the 1st step of the Workflow starts, Press the Black Cancel button located above the Workflow name.</t>
+  </si>
+  <si>
+    <t>As soon the step 1 ends the execution also ends and after a few seonds you are redirected to the results page. Validate the result page results.</t>
+  </si>
+  <si>
+    <t>The overal Workflow Execution status is "Cancelled by User".
+The step 1 was executed successfully, but the step 2 have the status "Cancelled by User"</t>
+  </si>
+  <si>
+    <t>Aborting a Workflow execution</t>
+  </si>
+  <si>
+    <t>As soon the 1st step of the Workflow starts, Press the Red "Kill it!" button located above the Workflow name.</t>
+  </si>
+  <si>
+    <t>A toast indicating the Workflow execution is cancellimng is displayed. Almost immediatelythe execution stops and you are redirected to the Results page</t>
+  </si>
+  <si>
+    <t>Check the execution report</t>
+  </si>
+  <si>
+    <t>The overal Workflow Execution status is "Cancelled by User".as the same status: "Cancelled by User"</t>
+  </si>
+  <si>
+    <t>You can upload the script successfully. This version of the script has the same second parameter named $Second. But in this case has no default value.</t>
+  </si>
+  <si>
+    <t>At the end of the execution in the Results page you can see the Step 3 finished sucessfully and now in the table of the results you can see a 2nd column named "$Second" that has no value.
+This is no causing issue, because this parametr is not required and can be null or empty.</t>
+  </si>
+  <si>
+    <t>Not Executed</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Create a new Workflow named "TestWorkflowHugeResults" and as descriiption "This workflow Exceeds the maximum data that can be stored in an execution results"
 Add the following steps:
@@ -628,12 +688,13 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">:
- -Name Step 1 30K results
+ -Name: Step 1 5K results
  -Script to execute: TestScript
  -Targets: Select 3 valid targets.
  - Script parameter changes:
     - $ResultType: JSON
-    - $TotalResults: 30000
+    - $TotalResults: 5000
+    - $ShowMessages: $false
 </t>
     </r>
     <r>
@@ -654,78 +715,19 @@
         <family val="2"/>
       </rPr>
       <t>:
- -Name Step 2 50K results
+ -Name: Step 2 20K results
  -Script to execute: TestScript
  -Targets: Select 3 valid targets.
  - Script parameter changes:
     - $ResultType: JSON
-    - $TotalResults: 50000
+    - $TotalResults: 20000
+    - $ShowMessages: $false
 Then click the Save &amp; Run button</t>
     </r>
   </si>
   <si>
-    <t>Review the Execution report</t>
-  </si>
-  <si>
-    <t>Creating and executing a Workflow that generates as huge Payload</t>
-  </si>
-  <si>
-    <t>Cancelling a Workflow execution</t>
-  </si>
-  <si>
-    <t>For the first step all the 30K results need to be there in a paginated Table.   
-For the second step, you need to see a legend saying the maximum quota for the results was exceeded and the data was discarded.</t>
-  </si>
-  <si>
-    <t>You are redirected to the Browse Workflows page where the Workflow TestWorkflowHugeResults is visible in the workflow list.</t>
-  </si>
-  <si>
-    <t>In the Search textbox of the navigation bar type the word "huge" and press enter.</t>
-  </si>
-  <si>
-    <t>Click the Run button at the right of the Workflow name</t>
-  </si>
-  <si>
-    <t>The workflow execution starts</t>
-  </si>
-  <si>
-    <t>As soon the 1st step of the Workflow starts, Press the Black Cancel button located above the Workflow name.</t>
-  </si>
-  <si>
-    <t>As soon the step 1 ends the execution also ends and after a few seonds you are redirected to the results page. Validate the result page results.</t>
-  </si>
-  <si>
-    <t>The overal Workflow Execution status is "Cancelled by User".
-The step 1 was executed successfully, but the step 2 have the status "Cancelled by User"</t>
-  </si>
-  <si>
-    <t>Aborting a Workflow execution</t>
-  </si>
-  <si>
-    <t>As soon the 1st step of the Workflow starts, Press the Red "Kill it!" button located above the Workflow name.</t>
-  </si>
-  <si>
-    <t>A toast indicating the Workflow execution is cancellimng is displayed. The Cancel button change his label to "Cancellation in progress…".
+    <t>A toast indicating the Workflow execution is cancelling is displayed. The Cancel button change his label to "Cancellation in progress…".
 Both Cancel and KillIt! Buttons are now disabled.</t>
-  </si>
-  <si>
-    <t>A toast indicating the Workflow execution is cancellimng is displayed. Almost immediatelythe execution stops and you are redirected to the Results page</t>
-  </si>
-  <si>
-    <t>Check the execution report</t>
-  </si>
-  <si>
-    <t>The overal Workflow Execution status is "Cancelled by User".as the same status: "Cancelled by User"</t>
-  </si>
-  <si>
-    <t>You can upload the script successfully. This version of the script has the same second parameter named $Second. But in this case has no default value.</t>
-  </si>
-  <si>
-    <t>At the end of the execution in the Results page you can see the Step 3 finished sucessfully and now in the table of the results you can see a 2nd column named "$Second" that has no value.
-This is no causing issue, because this parametr is not required and can be null or empty.</t>
-  </si>
-  <si>
-    <t>Not Executed</t>
   </si>
 </sst>
 </file>
@@ -4508,7 +4510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1510635-E20C-4AD1-9756-3BB17945F573}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -4764,7 +4766,7 @@
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -4783,7 +4785,7 @@
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4802,7 +4804,7 @@
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -4821,7 +4823,7 @@
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -4840,7 +4842,7 @@
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4859,7 +4861,7 @@
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -4878,7 +4880,7 @@
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -4897,7 +4899,7 @@
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -4916,7 +4918,7 @@
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -4935,7 +4937,7 @@
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -4954,7 +4956,7 @@
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -4973,7 +4975,7 @@
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="104" x14ac:dyDescent="0.35">
@@ -4992,7 +4994,7 @@
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="104" x14ac:dyDescent="0.35">
@@ -5011,7 +5013,7 @@
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -5030,7 +5032,7 @@
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="143" x14ac:dyDescent="0.35">
@@ -5049,7 +5051,7 @@
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -5271,7 +5273,7 @@
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5290,7 +5292,7 @@
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5309,7 +5311,7 @@
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -5328,7 +5330,7 @@
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="65" x14ac:dyDescent="0.35">
@@ -5347,7 +5349,7 @@
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5366,7 +5368,7 @@
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5385,7 +5387,7 @@
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5404,7 +5406,7 @@
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -5423,7 +5425,7 @@
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -5442,7 +5444,7 @@
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="65" x14ac:dyDescent="0.35">
@@ -5461,7 +5463,7 @@
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5480,7 +5482,7 @@
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5499,7 +5501,7 @@
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5518,7 +5520,7 @@
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -5537,7 +5539,7 @@
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="65" x14ac:dyDescent="0.35">
@@ -5556,7 +5558,7 @@
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5575,7 +5577,7 @@
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5594,7 +5596,7 @@
       </c>
       <c r="E28" s="21"/>
       <c r="F28" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="104" x14ac:dyDescent="0.35">
@@ -5613,7 +5615,7 @@
       </c>
       <c r="E29" s="21"/>
       <c r="F29" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -5632,7 +5634,7 @@
       </c>
       <c r="E30" s="21"/>
       <c r="F30" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -5863,7 +5865,7 @@
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5882,7 +5884,7 @@
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5901,7 +5903,7 @@
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5920,7 +5922,7 @@
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -5939,7 +5941,7 @@
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5958,7 +5960,7 @@
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -5977,7 +5979,7 @@
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="65" x14ac:dyDescent="0.35">
@@ -5996,7 +5998,7 @@
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -6015,7 +6017,7 @@
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -6034,7 +6036,7 @@
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -6053,7 +6055,7 @@
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -6068,11 +6070,11 @@
         <v>96</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -6091,7 +6093,7 @@
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="78" x14ac:dyDescent="0.35">
@@ -6106,11 +6108,11 @@
         <v>97</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -6129,7 +6131,7 @@
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -6148,7 +6150,7 @@
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -6167,7 +6169,7 @@
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -6186,7 +6188,7 @@
       </c>
       <c r="E28" s="21"/>
       <c r="F28" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -6205,7 +6207,7 @@
       </c>
       <c r="E29" s="21"/>
       <c r="F29" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="130" x14ac:dyDescent="0.35">
@@ -6224,7 +6226,7 @@
       </c>
       <c r="E30" s="21"/>
       <c r="F30" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -6243,7 +6245,7 @@
       </c>
       <c r="E31" s="21"/>
       <c r="F31" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6262,7 +6264,7 @@
       </c>
       <c r="E32" s="21"/>
       <c r="F32" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6281,7 +6283,7 @@
       </c>
       <c r="E33" s="17"/>
       <c r="F33" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="65" x14ac:dyDescent="0.35">
@@ -6300,7 +6302,7 @@
       </c>
       <c r="E34" s="17"/>
       <c r="F34" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6319,7 +6321,7 @@
       </c>
       <c r="E35" s="17"/>
       <c r="F35" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6338,7 +6340,7 @@
       </c>
       <c r="E36" s="17"/>
       <c r="F36" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -6357,7 +6359,7 @@
       </c>
       <c r="E37" s="17"/>
       <c r="F37" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -6376,7 +6378,7 @@
       </c>
       <c r="E38" s="17"/>
       <c r="F38" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="65" x14ac:dyDescent="0.35">
@@ -6395,7 +6397,7 @@
       </c>
       <c r="E39" s="17"/>
       <c r="F39" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6414,7 +6416,7 @@
       </c>
       <c r="E40" s="21"/>
       <c r="F40" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6433,7 +6435,7 @@
       </c>
       <c r="E41" s="21"/>
       <c r="F41" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6452,7 +6454,7 @@
       </c>
       <c r="E42" s="21"/>
       <c r="F42" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -6471,7 +6473,7 @@
       </c>
       <c r="E43" s="21"/>
       <c r="F43" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -6490,7 +6492,7 @@
       </c>
       <c r="E44" s="21"/>
       <c r="F44" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -6509,7 +6511,7 @@
       </c>
       <c r="E45" s="21"/>
       <c r="F45" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="78" x14ac:dyDescent="0.35">
@@ -6528,7 +6530,7 @@
       </c>
       <c r="E46" s="21"/>
       <c r="F46" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -6643,8 +6645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F494EF-1551-40A5-8DBA-63D5EE5106AF}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6781,7 +6783,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>19</v>
@@ -6791,26 +6793,26 @@
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="260" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="286" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>137</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="65" x14ac:dyDescent="0.35">
@@ -6819,17 +6821,17 @@
         <v>3</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -6838,17 +6840,17 @@
         <v>4</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6857,17 +6859,17 @@
         <v>5</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C15" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>145</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>146</v>
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="65" x14ac:dyDescent="0.35">
@@ -6876,17 +6878,17 @@
         <v>6</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -6895,17 +6897,17 @@
         <v>7</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C17" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>148</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>149</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -6914,17 +6916,17 @@
         <v>8</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="26" x14ac:dyDescent="0.35">
@@ -6933,17 +6935,17 @@
         <v>9</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C19" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>145</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>146</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="52" x14ac:dyDescent="0.35">
@@ -6952,17 +6954,17 @@
         <v>10</v>
       </c>
       <c r="B20" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C20" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="D20" s="10" t="s">
         <v>151</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>153</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="39" x14ac:dyDescent="0.35">
@@ -6971,17 +6973,17 @@
         <v>11</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>